<commit_message>
1. donat charts with echart4 2. first version of table
</commit_message>
<xml_diff>
--- a/ico_project.xlsx
+++ b/ico_project.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Common" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="270">
   <si>
     <t>Country</t>
   </si>
@@ -323,9 +323,6 @@
     <t>токены, которые можно использовать для доступа к определенному продукту или услуге, обычно предоставляемым с помощью платформы DLT</t>
   </si>
   <si>
-    <t>биржеыве токены</t>
-  </si>
-  <si>
     <t xml:space="preserve">токены, которые часто называют криптовалютами, они используют технологию распределенного хранения данных и не выпускаются и не поддерживаются Центральным банком или другим центральным органом. Они не предоставляют типы права или доступ к услугам и товарам, которые харктерны для утилити токенов  и токенов ценных бумаг, но используются в качестве средства обмена или для инвестиций. </t>
   </si>
   <si>
@@ -351,9 +348,6 @@
   </si>
   <si>
     <t>цифровые представления ценности, которая не была выпущена или гарантирована каким-либо Центральным банком или государственным органом и которая не имеет правового статуса валюты или денег, но которая принимается в качестве средства обмена или платежа или для инвестиционных целей любым физическим или юридическим лицом на основе соглашения или в соответствии с рыночной практикой и которая может передаваться, храниться и продаваться в электронном виде.</t>
-  </si>
-  <si>
-    <t>средство платежа (units of account)</t>
   </si>
   <si>
     <t>https://www.bafin.de/EN/Aufsicht/BankenFinanzdienstleister/Zulassung/Kryptoverwahrgeschaeft/kryptoverwahrgeschaeft_node_en.html</t>
@@ -740,9 +734,6 @@
     <t>Эмитенты утилити токенов могут получить лицензию во Французском Управлении Финансовым рынками (AMF). Лицензия даёт право компании открыть банковский счёт. Получение лицензии означает соблюдение всех требований безопасности и противодействия отмыванию денежных средств. Таким ICO компании попадают в так называемый "белый лист" ICO компаний Франции, который публикуется регулятором.</t>
   </si>
   <si>
-    <t>цифроой актив</t>
-  </si>
-  <si>
     <t>цифровое представление стоимости, которое не выдается или не гарантируется Центральным банком или государственным органом, которое не обязательно прикреплено к валюте, находящейся в законном обороте, но которое принимается физическими или юридическими лицами в качестве средства обмена и которое может быть передано, сохранено или обменено в электронном виде.</t>
   </si>
   <si>
@@ -762,6 +753,109 @@
   </si>
   <si>
     <t>национальное право</t>
+  </si>
+  <si>
+    <t>биржевые токены</t>
+  </si>
+  <si>
+    <t>цифровой актив</t>
+  </si>
+  <si>
+    <t>Австрия</t>
+  </si>
+  <si>
+    <t>Токены ценные бумаги предоставляют денежное требование эмитенту либо на корпоративной основе (например, дивиденды), либо на договорной основе (например, погашение основной суммы долга/процентов по кредиту). Таким образом, они очень похожи на традиционные долговые обязательства или акции. Форма оплаты не имеет значения (фиатная валюта или криптовалюта).</t>
+  </si>
+  <si>
+    <t>Используются в связи с  потреблением определенных продуктов или услуг. Если токен может быть использован только для очень ограниченного спектра продуктов или услуг (например, на одной платформе) и если он не предоставляет никаких других прав, он выглядит очень похожим на ваучер и не подлежит никакому регулирующему режиму. Однако, если он также может быть использован для оплаты, необходимо учитывать регулирующие последствия, установленные для платежных токенов.</t>
+  </si>
+  <si>
+    <t>нематериальное имущество</t>
+  </si>
+  <si>
+    <t>Бельгия</t>
+  </si>
+  <si>
+    <t>инвестиционный токен</t>
+  </si>
+  <si>
+    <t>токены, предоставляющие права на получение дохода</t>
+  </si>
+  <si>
+    <t>средство хранения, расчета и обмена, учитывая его конвертируемость в другие токены, криптовалюты или фиатные деньги</t>
+  </si>
+  <si>
+    <t>токен, который предоставляет к продукту или услуге</t>
+  </si>
+  <si>
+    <t>Италия</t>
+  </si>
+  <si>
+    <t>платежные токены в первую очередь выполняют платежную функцию для большей группы лиц. Для выпуска платежных токенов может потребоваться банковская лицензия (выпуск платежных средств), лицензия в соответствии с Законом об электронных деньгах или лицензия в соответствии с Законом о платежных услугах.</t>
+  </si>
+  <si>
+    <t>цифровое представление стоимости, не выпущенное центральным банком или государственным органом, не обязательно связанное с законным платежным средством, используемое в качестве средства обмена для покупки товаров и услуг и передаваемое, хранящееся в электронном виде</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cоздан единый реестр конечных бенефициарных собственников предприятий и трастов. В частности, специальный раздел Реестра предприятий является инструментом сбора и хранения информации о бенефициарных владельцах юридических лиц. Директора всех юридических лиц обязаны предоставлять в реестр соответствующую информацию и данные. В случае бездействия или необоснованного отказа акционера предоставить необходимую информацию его право голоса, связанное с пакетами акций, принадлежащими бенефициарному владельцу, будут заморожены. </t>
+  </si>
+  <si>
+    <t>Платформа обмена криптоактивами</t>
+  </si>
+  <si>
+    <t>токены, которые предоставляют права и обязательства, схожие с  акциями или долговыми инструментами (облигаций и других видов секьюритизированных долговых обязательств, производные финансовые контракты, паи в коллективных инвестиционных фондах и т.д.)</t>
+  </si>
+  <si>
+    <t>Зарегистрировать выпуск токенов активов в Службе финансового надзора; опубликовать проспект эмиссии; 
+идентифицировать покупателей токенов;</t>
+  </si>
+  <si>
+    <t>Польша</t>
+  </si>
+  <si>
+    <t>цифровое представление стоимости, которая не является: а) законным платежным средством, выпущенным НБП (Национальным банком Польши), иностранными центральными банками или другими органами государственного управления; б) международной клиринговой единицей, учрежденной международной организацией и принятой отдельными странами, входящими в такую организацию или сотрудничающими с ней; в) электронными деньгами по смыслу Закона от 19 августа 2011 года о платежных услугах; г) финансовым инструментом по смыслу Закона от 29 июля 2005 года о торговле финансовыми инструментами.; д) векселем или чеком. Конвертируется в коммерческих сделках в законные платежные средства и принимается в качестве средства обмена, а также может храниться или передаваться в электронном виде или может быть объектом электронной торговли</t>
+  </si>
+  <si>
+    <t>Специальных разъяснений о порядке опредлеения токена как финансового инструмента не даётся. Указывается, что токен, являющийся финансовым инструментом по смыслу польского законодательства и законодательства Европйского союза будет являться токеном ценной бумагой.</t>
+  </si>
+  <si>
+    <t>Швеция</t>
+  </si>
+  <si>
+    <t>Испания</t>
+  </si>
+  <si>
+    <t>не указано</t>
+  </si>
+  <si>
+    <t>цифровое представление стоимости, которое не выпущено или не гарантировано центральным банком или государственным органом, не обязательно привязано к законно установленной валюте и не обладает правовым статусом валюты или денег, но принимается физическими или юридическими лицами в качестве средства обмена и может передаваться, храниться и продаваться в электронном виде.</t>
+  </si>
+  <si>
+    <t>валютный токен</t>
+  </si>
+  <si>
+    <t>Утилити токены функционируют в основном либо как платежное средство в конкретной обстановке без использования в качестве общего платежного средства (например, оплата услуг или товаров от конкретного поставщика), либо как предоставление доступа к услуге или продукту через владение такими токенами.</t>
+  </si>
+  <si>
+    <t>не определено</t>
+  </si>
+  <si>
+    <t>токены, которые дают право на доступ к услуге или на получение продукта, без  упоминания  о повышении курса и ожиданиях ликвидности или о возможности торговли ими на конкретных рынках</t>
+  </si>
+  <si>
+    <t>токены, которые дают права или ожидание доли в потенциальном увеличении стоимости или прибыльности бизнеса или проектов или они представляют собой или присваивают права, эквивалентные или аналогичные правам акций, облигаций или других финансовых инструментов, регулируемых испанским законодательством о ценных бумагах</t>
+  </si>
+  <si>
+    <t>цифровое представление стоимости, которое не выпускается и не гарантируется центральным банком или государственным органом, не обязательно привязано к законно установленной валюте и не обладает правовым статусом валюты или денег, но принимается физическими или юридическими лицами в качестве средства обмена и может передаваться, храниться и продаваться в электронном виде.</t>
+  </si>
+  <si>
+    <t>Инвестиционные токены-это токены, основной целью которых является инвестирование, и обычно они дают финансовые права, а в некоторых случаях и права участия, аналогичные акциям компании</t>
+  </si>
+  <si>
+    <t>Норвегия</t>
+  </si>
+  <si>
+    <t>Португалия</t>
   </si>
 </sst>
 </file>
@@ -1192,10 +1286,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z12"/>
+  <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1310,7 +1404,7 @@
     </row>
     <row r="2" spans="1:26" ht="270" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>26</v>
@@ -1328,10 +1422,10 @@
         <v>28</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>29</v>
@@ -1352,10 +1446,10 @@
         <v>33</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>27</v>
@@ -1387,7 +1481,7 @@
     </row>
     <row r="3" spans="1:26" ht="225" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>26</v>
@@ -1464,7 +1558,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>26</v>
@@ -1503,10 +1597,10 @@
         <v>28</v>
       </c>
       <c r="N4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="O4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="P4" t="s">
         <v>28</v>
@@ -1533,7 +1627,7 @@
         <v>28</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="Z4" t="s">
         <v>53</v>
@@ -1541,7 +1635,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>26</v>
@@ -1610,7 +1704,7 @@
         <v>28</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="Z5" t="s">
         <v>62</v>
@@ -1618,7 +1712,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>64</v>
@@ -1660,7 +1754,7 @@
         <v>71</v>
       </c>
       <c r="O6" t="s">
-        <v>28</v>
+        <v>259</v>
       </c>
       <c r="P6" t="s">
         <v>72</v>
@@ -1687,7 +1781,7 @@
         <v>27</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Z6" t="s">
         <v>73</v>
@@ -1695,7 +1789,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>64</v>
@@ -1769,7 +1863,7 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>64</v>
@@ -1811,7 +1905,7 @@
         <v>71</v>
       </c>
       <c r="O8" t="s">
-        <v>28</v>
+        <v>259</v>
       </c>
       <c r="P8" t="s">
         <v>72</v>
@@ -1838,7 +1932,7 @@
         <v>27</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Z8" t="s">
         <v>85</v>
@@ -1846,7 +1940,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>26</v>
@@ -1915,7 +2009,7 @@
         <v>27</v>
       </c>
       <c r="X9" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Z9" s="1" t="s">
         <v>94</v>
@@ -1923,7 +2017,7 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>64</v>
@@ -1947,25 +2041,25 @@
         <v>95</v>
       </c>
       <c r="I10" t="s">
+        <v>236</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>83</v>
       </c>
       <c r="L10" t="s">
+        <v>97</v>
+      </c>
+      <c r="M10" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" t="s">
         <v>98</v>
       </c>
-      <c r="M10" t="s">
-        <v>27</v>
-      </c>
-      <c r="N10" t="s">
-        <v>99</v>
-      </c>
       <c r="O10" t="s">
-        <v>28</v>
+        <v>259</v>
       </c>
       <c r="P10" t="s">
         <v>93</v>
@@ -1992,15 +2086,15 @@
         <v>27</v>
       </c>
       <c r="X10" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z10" t="s">
         <v>100</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>64</v>
@@ -2021,28 +2115,28 @@
         <v>65</v>
       </c>
       <c r="H11" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I11" t="s">
         <v>103</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="K11" t="s">
+        <v>103</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="M11" t="s">
         <v>27</v>
       </c>
       <c r="N11" t="s">
-        <v>106</v>
+        <v>71</v>
       </c>
       <c r="O11" t="s">
-        <v>28</v>
+        <v>259</v>
       </c>
       <c r="P11" t="s">
         <v>93</v>
@@ -2069,15 +2163,15 @@
         <v>27</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Z11" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>26</v>
@@ -2095,28 +2189,28 @@
         <v>28</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>234</v>
-      </c>
       <c r="M12" t="s">
         <v>27</v>
       </c>
       <c r="P12" t="s">
-        <v>28</v>
+        <v>259</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>27</v>
@@ -2131,7 +2225,461 @@
         <v>27</v>
       </c>
       <c r="X12" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="I13" t="s">
+        <v>67</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="N13" t="s">
+        <v>241</v>
+      </c>
+      <c r="O13" t="s">
+        <v>259</v>
+      </c>
+      <c r="P13" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M14" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14" t="s">
+        <v>71</v>
+      </c>
+      <c r="O14" t="s">
+        <v>259</v>
+      </c>
+      <c r="P14" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="N15" t="s">
+        <v>71</v>
+      </c>
+      <c r="O15" t="s">
+        <v>259</v>
+      </c>
+      <c r="P15" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="N16" t="s">
+        <v>98</v>
+      </c>
+      <c r="O16" t="s">
+        <v>259</v>
+      </c>
+      <c r="P16" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="N17" t="s">
+        <v>71</v>
+      </c>
+      <c r="O17" t="s">
+        <v>259</v>
+      </c>
+      <c r="P17" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X17" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="M18" t="s">
+        <v>27</v>
+      </c>
+      <c r="N18" t="s">
+        <v>71</v>
+      </c>
+      <c r="O18" t="s">
+        <v>259</v>
+      </c>
+      <c r="P18" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X18" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -2139,16 +2687,16 @@
     <hyperlink ref="Z11" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2173,111 +2721,111 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" t="s">
         <v>116</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" t="s">
         <v>117</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>28</v>
@@ -2292,49 +2840,49 @@
         <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="J3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="P3" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>28</v>
@@ -2351,7 +2899,7 @@
         <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>28</v>
@@ -2408,49 +2956,49 @@
         <v>54</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="J5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K5" t="s">
-        <v>27</v>
-      </c>
-      <c r="L5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="P5" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="Q5" t="s">
         <v>28</v>
@@ -2465,49 +3013,49 @@
         <v>63</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="O6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="J6" t="s">
-        <v>28</v>
-      </c>
-      <c r="K6" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" t="s">
-        <v>27</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="Q6" t="s">
         <v>28</v>
@@ -2522,61 +3070,61 @@
         <v>74</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J7" t="s">
+        <v>77</v>
+      </c>
+      <c r="K7" t="s">
+        <v>77</v>
+      </c>
+      <c r="L7" t="s">
+        <v>77</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="O7" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="J7" t="s">
-        <v>77</v>
-      </c>
-      <c r="K7" t="s">
-        <v>77</v>
-      </c>
-      <c r="L7" t="s">
-        <v>77</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>154</v>
-      </c>
       <c r="P7" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>77</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>77</v>
       </c>
       <c r="T7" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -2584,49 +3132,49 @@
         <v>80</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="O8" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" t="s">
-        <v>28</v>
-      </c>
-      <c r="K8" t="s">
-        <v>28</v>
-      </c>
-      <c r="L8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="Q8" t="s">
         <v>28</v>
@@ -2644,46 +3192,46 @@
         <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="O9" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="P9" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" t="s">
-        <v>27</v>
-      </c>
-      <c r="K9" t="s">
-        <v>27</v>
-      </c>
-      <c r="L9" t="s">
-        <v>27</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="Q9" s="1" t="s">
         <v>27</v>
@@ -2695,52 +3243,52 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="E10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K10" t="s">
-        <v>28</v>
-      </c>
-      <c r="L10" t="s">
-        <v>27</v>
-      </c>
-      <c r="M10" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>28</v>
@@ -2751,16 +3299,16 @@
     </row>
     <row r="11" spans="1:20" ht="165" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>27</v>
@@ -2790,13 +3338,13 @@
         <v>28</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>28</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Q11" s="1" t="s">
         <v>28</v>
@@ -2807,36 +3355,375 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>230</v>
-      </c>
       <c r="Q12" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K16" t="s">
+        <v>28</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R18" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2848,10 +3735,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2873,63 +3760,63 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" t="s">
         <v>172</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G1" t="s">
+        <v>222</v>
+      </c>
+      <c r="H1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I1" t="s">
+        <v>218</v>
+      </c>
+      <c r="J1" t="s">
+        <v>220</v>
+      </c>
+      <c r="K1" t="s">
         <v>173</v>
       </c>
-      <c r="D1" t="s">
+      <c r="L1" t="s">
         <v>174</v>
       </c>
-      <c r="E1" t="s">
-        <v>226</v>
-      </c>
-      <c r="F1" t="s">
-        <v>225</v>
-      </c>
-      <c r="G1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H1" t="s">
-        <v>221</v>
-      </c>
-      <c r="I1" t="s">
-        <v>220</v>
-      </c>
-      <c r="J1" t="s">
-        <v>222</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>175</v>
-      </c>
-      <c r="L1" t="s">
-        <v>176</v>
-      </c>
-      <c r="M1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E2" t="s">
         <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H2" t="s">
         <v>28</v>
@@ -2938,7 +3825,7 @@
         <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="K2" t="s">
         <v>28</v>
@@ -2949,25 +3836,25 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H3" t="s">
         <v>28</v>
@@ -2976,7 +3863,7 @@
         <v>28</v>
       </c>
       <c r="J3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="K3" t="s">
         <v>28</v>
@@ -2987,22 +3874,22 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E4" t="s">
         <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G4" t="s">
         <v>77</v>
@@ -3014,7 +3901,7 @@
         <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="K4" t="s">
         <v>27</v>
@@ -3025,25 +3912,25 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E5" t="s">
         <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H5" t="s">
         <v>28</v>
@@ -3052,7 +3939,7 @@
         <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K5" t="s">
         <v>27</v>
@@ -3063,25 +3950,25 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E6" t="s">
         <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G6" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H6" t="s">
         <v>28</v>
@@ -3090,7 +3977,7 @@
         <v>28</v>
       </c>
       <c r="J6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K6" t="s">
         <v>27</v>
@@ -3101,25 +3988,25 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H7" t="s">
         <v>27</v>
@@ -3128,7 +4015,7 @@
         <v>27</v>
       </c>
       <c r="J7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="K7" t="s">
         <v>28</v>
@@ -3139,25 +4026,25 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E8" t="s">
         <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G8" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H8" t="s">
         <v>28</v>
@@ -3166,7 +4053,7 @@
         <v>28</v>
       </c>
       <c r="J8" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="K8" t="s">
         <v>27</v>
@@ -3177,25 +4064,25 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D9" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E9" t="s">
         <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G9" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H9" t="s">
         <v>27</v>
@@ -3204,7 +4091,7 @@
         <v>27</v>
       </c>
       <c r="J9" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="K9" t="s">
         <v>28</v>
@@ -3215,25 +4102,25 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E10" t="s">
         <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G10" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H10" t="s">
         <v>27</v>
@@ -3242,7 +4129,7 @@
         <v>28</v>
       </c>
       <c r="J10" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="K10" t="s">
         <v>27</v>
@@ -3253,39 +4140,272 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C11" t="s">
+        <v>235</v>
+      </c>
+      <c r="D11" t="s">
+        <v>176</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
+        <v>235</v>
+      </c>
+      <c r="G11" t="s">
+        <v>235</v>
+      </c>
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" t="s">
+        <v>176</v>
+      </c>
+      <c r="K11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="D11" t="s">
-        <v>178</v>
-      </c>
-      <c r="E11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" t="s">
-        <v>238</v>
-      </c>
-      <c r="G11" t="s">
-        <v>238</v>
-      </c>
-      <c r="H11" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" t="s">
-        <v>178</v>
-      </c>
-      <c r="K11" t="s">
-        <v>27</v>
-      </c>
-      <c r="L11" t="s">
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>235</v>
+      </c>
+      <c r="D13" t="s">
+        <v>176</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" t="s">
+        <v>235</v>
+      </c>
+      <c r="G13" t="s">
+        <v>235</v>
+      </c>
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" t="s">
+        <v>235</v>
+      </c>
+      <c r="K13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>235</v>
+      </c>
+      <c r="D14" t="s">
+        <v>176</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" t="s">
+        <v>235</v>
+      </c>
+      <c r="G14" t="s">
+        <v>235</v>
+      </c>
+      <c r="H14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" t="s">
+        <v>235</v>
+      </c>
+      <c r="K14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>235</v>
+      </c>
+      <c r="D15" t="s">
+        <v>176</v>
+      </c>
+      <c r="E15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" t="s">
+        <v>235</v>
+      </c>
+      <c r="G15" t="s">
+        <v>235</v>
+      </c>
+      <c r="H15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" t="s">
+        <v>28</v>
+      </c>
+      <c r="J15" t="s">
+        <v>235</v>
+      </c>
+      <c r="K15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>235</v>
+      </c>
+      <c r="D16" t="s">
+        <v>176</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" t="s">
+        <v>235</v>
+      </c>
+      <c r="G16" t="s">
+        <v>235</v>
+      </c>
+      <c r="H16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" t="s">
+        <v>28</v>
+      </c>
+      <c r="J16" t="s">
+        <v>235</v>
+      </c>
+      <c r="K16" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>235</v>
+      </c>
+      <c r="D17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" t="s">
+        <v>235</v>
+      </c>
+      <c r="G17" t="s">
+        <v>235</v>
+      </c>
+      <c r="H17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" t="s">
+        <v>235</v>
+      </c>
+      <c r="K17" t="s">
+        <v>27</v>
+      </c>
+      <c r="L17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>235</v>
+      </c>
+      <c r="D18" t="s">
+        <v>176</v>
+      </c>
+      <c r="E18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" t="s">
+        <v>235</v>
+      </c>
+      <c r="G18" t="s">
+        <v>235</v>
+      </c>
+      <c r="H18" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" t="s">
+        <v>28</v>
+      </c>
+      <c r="J18" t="s">
+        <v>235</v>
+      </c>
+      <c r="K18" t="s">
+        <v>27</v>
+      </c>
+      <c r="L18" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3297,10 +4417,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3320,30 +4440,30 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" t="s">
         <v>181</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>182</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>183</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>184</v>
-      </c>
-      <c r="F1" t="s">
-        <v>185</v>
-      </c>
-      <c r="G1" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>28</v>
@@ -3355,7 +4475,7 @@
         <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>28</v>
@@ -3524,7 +4644,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>28</v>
@@ -3547,7 +4667,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>28</v>
@@ -3566,6 +4686,16 @@
       </c>
       <c r="G11" s="1" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -3576,10 +4706,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:W13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3609,72 +4739,72 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G1" t="s">
+        <v>198</v>
+      </c>
+      <c r="H1" t="s">
+        <v>199</v>
+      </c>
+      <c r="I1" t="s">
+        <v>200</v>
+      </c>
+      <c r="J1" t="s">
+        <v>201</v>
+      </c>
+      <c r="K1" t="s">
+        <v>202</v>
+      </c>
+      <c r="L1" t="s">
+        <v>208</v>
+      </c>
+      <c r="M1" t="s">
         <v>205</v>
       </c>
-      <c r="C1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="N1" t="s">
+        <v>217</v>
+      </c>
+      <c r="O1" t="s">
         <v>209</v>
       </c>
-      <c r="E1" t="s">
-        <v>206</v>
-      </c>
-      <c r="F1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G1" t="s">
-        <v>200</v>
-      </c>
-      <c r="H1" t="s">
-        <v>201</v>
-      </c>
-      <c r="I1" t="s">
-        <v>202</v>
-      </c>
-      <c r="J1" t="s">
-        <v>203</v>
-      </c>
-      <c r="K1" t="s">
-        <v>204</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>210</v>
       </c>
-      <c r="M1" t="s">
-        <v>207</v>
-      </c>
-      <c r="N1" t="s">
-        <v>219</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>211</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
+        <v>215</v>
+      </c>
+      <c r="S1" t="s">
         <v>212</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
+        <v>214</v>
+      </c>
+      <c r="U1" t="s">
         <v>213</v>
       </c>
-      <c r="R1" t="s">
-        <v>217</v>
-      </c>
-      <c r="S1" t="s">
-        <v>214</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>216</v>
-      </c>
-      <c r="U1" t="s">
-        <v>215</v>
-      </c>
-      <c r="V1" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
         <v>77</v>
@@ -3742,7 +4872,7 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B3" s="8">
         <v>43090</v>
@@ -3810,7 +4940,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B4" s="8">
         <v>44007</v>
@@ -3878,7 +5008,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B5" s="8">
         <v>44134</v>
@@ -3943,7 +5073,7 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B6" s="8">
         <v>43546</v>
@@ -4011,7 +5141,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B7" t="s">
         <v>77</v>
@@ -4079,7 +5209,7 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B8" s="8">
         <v>43066</v>
@@ -4147,7 +5277,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B9" s="8">
         <v>42826</v>
@@ -4216,7 +5346,7 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B10" s="8">
         <v>43840</v>
@@ -4284,7 +5414,7 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B11" s="8">
         <v>43784</v>
@@ -4348,6 +5478,16 @@
       </c>
       <c r="V11" s="8">
         <v>43187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>